<commit_message>
update cases, addet status
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="674">
   <si>
     <t>№</t>
   </si>
@@ -35247,24 +35247,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -35274,14 +35256,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -35565,8 +35565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C152" sqref="C152"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I156" sqref="I156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35616,7 +35616,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="70" t="s">
         <v>82</v>
       </c>
       <c r="B2" s="40">
@@ -35644,7 +35644,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="77"/>
+      <c r="A3" s="71"/>
       <c r="B3" s="40">
         <v>2</v>
       </c>
@@ -35670,7 +35670,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="78"/>
+      <c r="A4" s="72"/>
       <c r="B4" s="40">
         <v>3</v>
       </c>
@@ -35696,7 +35696,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="76" t="s">
         <v>85</v>
       </c>
       <c r="B5" s="4">
@@ -35724,7 +35724,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="74"/>
+      <c r="A6" s="77"/>
       <c r="B6" s="6">
         <v>5</v>
       </c>
@@ -35750,7 +35750,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="74"/>
+      <c r="A7" s="77"/>
       <c r="B7" s="6">
         <v>6</v>
       </c>
@@ -35778,7 +35778,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="74"/>
+      <c r="A8" s="77"/>
       <c r="B8" s="6">
         <v>7</v>
       </c>
@@ -35804,7 +35804,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="74"/>
+      <c r="A9" s="77"/>
       <c r="B9" s="6">
         <v>8</v>
       </c>
@@ -35830,7 +35830,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="74"/>
+      <c r="A10" s="77"/>
       <c r="B10" s="6">
         <v>9</v>
       </c>
@@ -35856,7 +35856,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="74"/>
+      <c r="A11" s="77"/>
       <c r="B11" s="6">
         <v>10</v>
       </c>
@@ -35882,7 +35882,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="74"/>
+      <c r="A12" s="77"/>
       <c r="B12" s="6">
         <v>11</v>
       </c>
@@ -35908,7 +35908,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="61.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="81"/>
+      <c r="A13" s="78"/>
       <c r="B13" s="45">
         <v>12</v>
       </c>
@@ -35934,7 +35934,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="73" t="s">
         <v>113</v>
       </c>
       <c r="B14" s="12">
@@ -35962,7 +35962,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="71"/>
+      <c r="A15" s="74"/>
       <c r="B15" s="17">
         <v>14</v>
       </c>
@@ -35988,7 +35988,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="71"/>
+      <c r="A16" s="74"/>
       <c r="B16" s="17">
         <v>15</v>
       </c>
@@ -36014,7 +36014,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="82.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="80"/>
+      <c r="A17" s="75"/>
       <c r="B17" s="45">
         <v>16</v>
       </c>
@@ -36040,7 +36040,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="76" t="s">
+      <c r="A18" s="70" t="s">
         <v>128</v>
       </c>
       <c r="B18" s="20">
@@ -36068,7 +36068,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="77"/>
+      <c r="A19" s="71"/>
       <c r="B19" s="17">
         <v>18</v>
       </c>
@@ -36094,7 +36094,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="77"/>
+      <c r="A20" s="71"/>
       <c r="B20" s="18">
         <v>19</v>
       </c>
@@ -36120,7 +36120,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="77"/>
+      <c r="A21" s="71"/>
       <c r="B21" s="18">
         <v>20</v>
       </c>
@@ -36146,7 +36146,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="77"/>
+      <c r="A22" s="71"/>
       <c r="B22" s="18">
         <v>21</v>
       </c>
@@ -36172,7 +36172,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="77"/>
+      <c r="A23" s="71"/>
       <c r="B23" s="18">
         <v>22</v>
       </c>
@@ -36198,7 +36198,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="77"/>
+      <c r="A24" s="71"/>
       <c r="B24" s="47">
         <v>23</v>
       </c>
@@ -36224,7 +36224,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="70" t="s">
+      <c r="A25" s="73" t="s">
         <v>157</v>
       </c>
       <c r="B25" s="13">
@@ -36252,7 +36252,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="71"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="18">
         <v>25</v>
       </c>
@@ -36278,7 +36278,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="71"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="18">
         <v>26</v>
       </c>
@@ -36304,7 +36304,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="82.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="80"/>
+      <c r="A28" s="75"/>
       <c r="B28" s="21">
         <v>27</v>
       </c>
@@ -36330,7 +36330,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="70" t="s">
+      <c r="A29" s="73" t="s">
         <v>170</v>
       </c>
       <c r="B29" s="13">
@@ -36358,7 +36358,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="71"/>
+      <c r="A30" s="74"/>
       <c r="B30" s="18">
         <v>29</v>
       </c>
@@ -36384,7 +36384,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="71"/>
+      <c r="A31" s="74"/>
       <c r="B31" s="18">
         <v>30</v>
       </c>
@@ -36410,7 +36410,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="71"/>
+      <c r="A32" s="74"/>
       <c r="B32" s="18">
         <v>31</v>
       </c>
@@ -36436,7 +36436,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="71"/>
+      <c r="A33" s="74"/>
       <c r="B33" s="18">
         <v>32</v>
       </c>
@@ -36462,7 +36462,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="61.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="80"/>
+      <c r="A34" s="75"/>
       <c r="B34" s="21">
         <v>33</v>
       </c>
@@ -36488,7 +36488,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="70" t="s">
+      <c r="A35" s="73" t="s">
         <v>189</v>
       </c>
       <c r="B35" s="13">
@@ -36516,7 +36516,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="71"/>
+      <c r="A36" s="74"/>
       <c r="B36" s="18">
         <v>35</v>
       </c>
@@ -36542,7 +36542,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="71"/>
+      <c r="A37" s="74"/>
       <c r="B37" s="18">
         <v>36</v>
       </c>
@@ -36568,7 +36568,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="71"/>
+      <c r="A38" s="74"/>
       <c r="B38" s="18">
         <v>37</v>
       </c>
@@ -36594,7 +36594,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="71"/>
+      <c r="A39" s="74"/>
       <c r="B39" s="18">
         <v>38</v>
       </c>
@@ -36620,7 +36620,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="71"/>
+      <c r="A40" s="74"/>
       <c r="B40" s="18">
         <v>39</v>
       </c>
@@ -36646,7 +36646,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="80"/>
+      <c r="A41" s="75"/>
       <c r="B41" s="21">
         <v>40</v>
       </c>
@@ -36672,7 +36672,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="70" t="s">
+      <c r="A42" s="73" t="s">
         <v>211</v>
       </c>
       <c r="B42" s="13">
@@ -36700,7 +36700,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="71"/>
+      <c r="A43" s="74"/>
       <c r="B43" s="18">
         <v>42</v>
       </c>
@@ -36726,7 +36726,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="71"/>
+      <c r="A44" s="74"/>
       <c r="B44" s="18">
         <v>43</v>
       </c>
@@ -36752,7 +36752,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" ht="61.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="71"/>
+      <c r="A45" s="74"/>
       <c r="B45" s="18">
         <v>44</v>
       </c>
@@ -36778,7 +36778,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" ht="61.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="71"/>
+      <c r="A46" s="74"/>
       <c r="B46" s="18">
         <v>45</v>
       </c>
@@ -36804,7 +36804,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="61.2" x14ac:dyDescent="0.3">
-      <c r="A47" s="71"/>
+      <c r="A47" s="74"/>
       <c r="B47" s="18">
         <v>46</v>
       </c>
@@ -36830,7 +36830,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="71"/>
+      <c r="A48" s="74"/>
       <c r="B48" s="18">
         <v>47</v>
       </c>
@@ -36856,7 +36856,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="71"/>
+      <c r="A49" s="74"/>
       <c r="B49" s="18">
         <v>48</v>
       </c>
@@ -36882,7 +36882,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="61.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="80"/>
+      <c r="A50" s="75"/>
       <c r="B50" s="21">
         <v>49</v>
       </c>
@@ -36908,7 +36908,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="177" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="70" t="s">
+      <c r="A51" s="73" t="s">
         <v>225</v>
       </c>
       <c r="B51" s="13">
@@ -36938,7 +36938,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="71"/>
+      <c r="A52" s="74"/>
       <c r="B52" s="18">
         <v>51</v>
       </c>
@@ -36964,7 +36964,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="71"/>
+      <c r="A53" s="74"/>
       <c r="B53" s="18">
         <v>52</v>
       </c>
@@ -36990,7 +36990,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="71"/>
+      <c r="A54" s="74"/>
       <c r="B54" s="18">
         <v>53</v>
       </c>
@@ -37016,7 +37016,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="71"/>
+      <c r="A55" s="74"/>
       <c r="B55" s="18">
         <v>54</v>
       </c>
@@ -37042,7 +37042,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="71"/>
+      <c r="A56" s="74"/>
       <c r="B56" s="18">
         <v>55</v>
       </c>
@@ -37068,7 +37068,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="71"/>
+      <c r="A57" s="74"/>
       <c r="B57" s="18">
         <v>56</v>
       </c>
@@ -37092,7 +37092,7 @@
       <c r="J57" s="24"/>
     </row>
     <row r="58" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="71"/>
+      <c r="A58" s="74"/>
       <c r="B58" s="18">
         <v>57</v>
       </c>
@@ -37118,7 +37118,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="71"/>
+      <c r="A59" s="74"/>
       <c r="B59" s="18">
         <v>58</v>
       </c>
@@ -37144,7 +37144,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="71"/>
+      <c r="A60" s="74"/>
       <c r="B60" s="18">
         <v>59</v>
       </c>
@@ -37170,7 +37170,7 @@
       </c>
     </row>
     <row r="61" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="71"/>
+      <c r="A61" s="74"/>
       <c r="B61" s="6">
         <v>60</v>
       </c>
@@ -37194,7 +37194,7 @@
       <c r="J61" s="24"/>
     </row>
     <row r="62" spans="1:10" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="71"/>
+      <c r="A62" s="74"/>
       <c r="B62" s="6">
         <v>61</v>
       </c>
@@ -37218,7 +37218,7 @@
       <c r="J62" s="24"/>
     </row>
     <row r="63" spans="1:10" ht="46.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="80"/>
+      <c r="A63" s="75"/>
       <c r="B63" s="45">
         <v>62</v>
       </c>
@@ -37244,7 +37244,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="193.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="70" t="s">
+      <c r="A64" s="73" t="s">
         <v>268</v>
       </c>
       <c r="B64" s="13">
@@ -37274,7 +37274,7 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="71"/>
+      <c r="A65" s="74"/>
       <c r="B65" s="18">
         <v>64</v>
       </c>
@@ -37300,7 +37300,7 @@
       </c>
     </row>
     <row r="66" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="71"/>
+      <c r="A66" s="74"/>
       <c r="B66" s="18">
         <v>65</v>
       </c>
@@ -37326,7 +37326,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="71"/>
+      <c r="A67" s="74"/>
       <c r="B67" s="18">
         <v>66</v>
       </c>
@@ -37352,7 +37352,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="71"/>
+      <c r="A68" s="74"/>
       <c r="B68" s="18">
         <v>67</v>
       </c>
@@ -37376,7 +37376,7 @@
       <c r="J68" s="24"/>
     </row>
     <row r="69" spans="1:10" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="71"/>
+      <c r="A69" s="74"/>
       <c r="B69" s="18">
         <v>68</v>
       </c>
@@ -37400,7 +37400,7 @@
       <c r="J69" s="24"/>
     </row>
     <row r="70" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="71"/>
+      <c r="A70" s="74"/>
       <c r="B70" s="18">
         <v>69</v>
       </c>
@@ -37426,7 +37426,7 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="71"/>
+      <c r="A71" s="74"/>
       <c r="B71" s="18">
         <v>70</v>
       </c>
@@ -37452,7 +37452,7 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="71"/>
+      <c r="A72" s="74"/>
       <c r="B72" s="18">
         <v>71</v>
       </c>
@@ -37478,7 +37478,7 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="71"/>
+      <c r="A73" s="74"/>
       <c r="B73" s="6">
         <v>72</v>
       </c>
@@ -37502,7 +37502,7 @@
       <c r="J73" s="24"/>
     </row>
     <row r="74" spans="1:10" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="71"/>
+      <c r="A74" s="74"/>
       <c r="B74" s="6">
         <v>73</v>
       </c>
@@ -37526,7 +37526,7 @@
       <c r="J74" s="24"/>
     </row>
     <row r="75" spans="1:10" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="71"/>
+      <c r="A75" s="74"/>
       <c r="B75" s="6">
         <v>74</v>
       </c>
@@ -37552,7 +37552,7 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="71"/>
+      <c r="A76" s="74"/>
       <c r="B76" s="18">
         <v>75</v>
       </c>
@@ -37578,7 +37578,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="71"/>
+      <c r="A77" s="74"/>
       <c r="B77" s="18">
         <v>76</v>
       </c>
@@ -37604,7 +37604,7 @@
       </c>
     </row>
     <row r="78" spans="1:10" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="80"/>
+      <c r="A78" s="75"/>
       <c r="B78" s="21">
         <v>77</v>
       </c>
@@ -37630,7 +37630,7 @@
       </c>
     </row>
     <row r="79" spans="1:10" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="80"/>
+      <c r="A79" s="75"/>
       <c r="B79" s="22">
         <v>78</v>
       </c>
@@ -37656,7 +37656,7 @@
       </c>
     </row>
     <row r="80" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="70" t="s">
+      <c r="A80" s="73" t="s">
         <v>305</v>
       </c>
       <c r="B80" s="15">
@@ -37684,7 +37684,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="71"/>
+      <c r="A81" s="74"/>
       <c r="B81" s="18">
         <v>80</v>
       </c>
@@ -37710,7 +37710,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="80"/>
+      <c r="A82" s="75"/>
       <c r="B82" s="21">
         <v>81</v>
       </c>
@@ -37736,7 +37736,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="73" t="s">
+      <c r="A83" s="76" t="s">
         <v>564</v>
       </c>
       <c r="B83" s="13">
@@ -37764,7 +37764,7 @@
       </c>
     </row>
     <row r="84" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="74"/>
+      <c r="A84" s="77"/>
       <c r="B84" s="18">
         <v>83</v>
       </c>
@@ -37790,7 +37790,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="74"/>
+      <c r="A85" s="77"/>
       <c r="B85" s="18">
         <v>84</v>
       </c>
@@ -37816,7 +37816,7 @@
       </c>
     </row>
     <row r="86" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="74"/>
+      <c r="A86" s="77"/>
       <c r="B86" s="18">
         <v>85</v>
       </c>
@@ -37842,7 +37842,7 @@
       </c>
     </row>
     <row r="87" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="74"/>
+      <c r="A87" s="77"/>
       <c r="B87" s="18">
         <v>86</v>
       </c>
@@ -37868,7 +37868,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="74"/>
+      <c r="A88" s="77"/>
       <c r="B88" s="18">
         <v>87</v>
       </c>
@@ -37894,7 +37894,7 @@
       </c>
     </row>
     <row r="89" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="74"/>
+      <c r="A89" s="77"/>
       <c r="B89" s="18">
         <v>88</v>
       </c>
@@ -37920,7 +37920,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="74"/>
+      <c r="A90" s="77"/>
       <c r="B90" s="18">
         <v>89</v>
       </c>
@@ -37946,7 +37946,7 @@
       </c>
     </row>
     <row r="91" spans="1:10" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="75"/>
+      <c r="A91" s="80"/>
       <c r="B91" s="19">
         <v>90</v>
       </c>
@@ -37972,7 +37972,7 @@
       </c>
     </row>
     <row r="92" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="70" t="s">
+      <c r="A92" s="73" t="s">
         <v>599</v>
       </c>
       <c r="B92" s="13">
@@ -38000,7 +38000,7 @@
       </c>
     </row>
     <row r="93" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="71"/>
+      <c r="A93" s="74"/>
       <c r="B93" s="18">
         <v>92</v>
       </c>
@@ -38026,7 +38026,7 @@
       </c>
     </row>
     <row r="94" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="71"/>
+      <c r="A94" s="74"/>
       <c r="B94" s="18">
         <v>93</v>
       </c>
@@ -38052,7 +38052,7 @@
       </c>
     </row>
     <row r="95" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="71"/>
+      <c r="A95" s="74"/>
       <c r="B95" s="18">
         <v>94</v>
       </c>
@@ -38078,7 +38078,7 @@
       </c>
     </row>
     <row r="96" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="71"/>
+      <c r="A96" s="74"/>
       <c r="B96" s="18">
         <v>95</v>
       </c>
@@ -38104,7 +38104,7 @@
       </c>
     </row>
     <row r="97" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="71"/>
+      <c r="A97" s="74"/>
       <c r="B97" s="18">
         <v>96</v>
       </c>
@@ -38130,7 +38130,7 @@
       </c>
     </row>
     <row r="98" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="71"/>
+      <c r="A98" s="74"/>
       <c r="B98" s="18">
         <v>97</v>
       </c>
@@ -38154,7 +38154,7 @@
       <c r="J98" s="24"/>
     </row>
     <row r="99" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="71"/>
+      <c r="A99" s="74"/>
       <c r="B99" s="18">
         <v>98</v>
       </c>
@@ -38180,7 +38180,7 @@
       </c>
     </row>
     <row r="100" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="71"/>
+      <c r="A100" s="74"/>
       <c r="B100" s="18">
         <v>99</v>
       </c>
@@ -38206,7 +38206,7 @@
       </c>
     </row>
     <row r="101" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="71"/>
+      <c r="A101" s="74"/>
       <c r="B101" s="29">
         <v>100</v>
       </c>
@@ -38232,7 +38232,7 @@
       </c>
     </row>
     <row r="102" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="71"/>
+      <c r="A102" s="74"/>
       <c r="B102" s="62">
         <v>101</v>
       </c>
@@ -38256,7 +38256,7 @@
       <c r="J102" s="24"/>
     </row>
     <row r="103" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="71"/>
+      <c r="A103" s="74"/>
       <c r="B103" s="62">
         <v>102</v>
       </c>
@@ -38280,7 +38280,7 @@
       <c r="J103" s="24"/>
     </row>
     <row r="104" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="71"/>
+      <c r="A104" s="74"/>
       <c r="B104" s="62">
         <v>103</v>
       </c>
@@ -38306,7 +38306,7 @@
       </c>
     </row>
     <row r="105" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="71"/>
+      <c r="A105" s="74"/>
       <c r="B105" s="29">
         <v>104</v>
       </c>
@@ -38332,7 +38332,7 @@
       </c>
     </row>
     <row r="106" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="71"/>
+      <c r="A106" s="74"/>
       <c r="B106" s="29">
         <v>105</v>
       </c>
@@ -38358,7 +38358,7 @@
       </c>
     </row>
     <row r="107" spans="1:10" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="72"/>
+      <c r="A107" s="79"/>
       <c r="B107" s="31">
         <v>106</v>
       </c>
@@ -38384,7 +38384,7 @@
       </c>
     </row>
     <row r="108" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="79" t="s">
+      <c r="A108" s="81" t="s">
         <v>314</v>
       </c>
       <c r="B108" s="63">
@@ -38412,7 +38412,7 @@
       </c>
     </row>
     <row r="109" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="71"/>
+      <c r="A109" s="74"/>
       <c r="B109" s="29">
         <v>108</v>
       </c>
@@ -38438,7 +38438,7 @@
       </c>
     </row>
     <row r="110" spans="1:10" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="71"/>
+      <c r="A110" s="74"/>
       <c r="B110" s="29">
         <v>109</v>
       </c>
@@ -38466,7 +38466,7 @@
       </c>
     </row>
     <row r="111" spans="1:10" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="71"/>
+      <c r="A111" s="74"/>
       <c r="B111" s="29">
         <v>110</v>
       </c>
@@ -38492,7 +38492,7 @@
       </c>
     </row>
     <row r="112" spans="1:10" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="71"/>
+      <c r="A112" s="74"/>
       <c r="B112" s="29">
         <v>111</v>
       </c>
@@ -38516,7 +38516,7 @@
       <c r="J112" s="24"/>
     </row>
     <row r="113" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="71"/>
+      <c r="A113" s="74"/>
       <c r="B113" s="29">
         <v>112</v>
       </c>
@@ -38542,7 +38542,7 @@
       </c>
     </row>
     <row r="114" spans="1:10" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="71"/>
+      <c r="A114" s="74"/>
       <c r="B114" s="29">
         <v>113</v>
       </c>
@@ -38566,7 +38566,7 @@
       <c r="J114" s="24"/>
     </row>
     <row r="115" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="71"/>
+      <c r="A115" s="74"/>
       <c r="B115" s="29">
         <v>114</v>
       </c>
@@ -38592,7 +38592,7 @@
       </c>
     </row>
     <row r="116" spans="1:10" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="71"/>
+      <c r="A116" s="74"/>
       <c r="B116" s="30">
         <v>115</v>
       </c>
@@ -38618,7 +38618,7 @@
       </c>
     </row>
     <row r="117" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="71"/>
+      <c r="A117" s="74"/>
       <c r="B117" s="62">
         <v>116</v>
       </c>
@@ -38644,7 +38644,7 @@
       </c>
     </row>
     <row r="118" spans="1:10" ht="61.2" x14ac:dyDescent="0.3">
-      <c r="A118" s="71"/>
+      <c r="A118" s="74"/>
       <c r="B118" s="62">
         <v>117</v>
       </c>
@@ -38670,7 +38670,7 @@
       </c>
     </row>
     <row r="119" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="71"/>
+      <c r="A119" s="74"/>
       <c r="B119" s="62">
         <v>118</v>
       </c>
@@ -38696,7 +38696,7 @@
       </c>
     </row>
     <row r="120" spans="1:10" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="71"/>
+      <c r="A120" s="74"/>
       <c r="B120" s="62">
         <v>119</v>
       </c>
@@ -38722,7 +38722,7 @@
       </c>
     </row>
     <row r="121" spans="1:10" ht="61.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="80"/>
+      <c r="A121" s="75"/>
       <c r="B121" s="64">
         <v>120</v>
       </c>
@@ -38748,7 +38748,7 @@
       </c>
     </row>
     <row r="122" spans="1:10" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A122" s="70" t="s">
+      <c r="A122" s="73" t="s">
         <v>345</v>
       </c>
       <c r="B122" s="32">
@@ -38776,7 +38776,7 @@
       </c>
     </row>
     <row r="123" spans="1:10" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A123" s="71"/>
+      <c r="A123" s="74"/>
       <c r="B123" s="29">
         <v>122</v>
       </c>
@@ -38802,7 +38802,7 @@
       </c>
     </row>
     <row r="124" spans="1:10" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A124" s="71"/>
+      <c r="A124" s="74"/>
       <c r="B124" s="29">
         <v>123</v>
       </c>
@@ -38828,7 +38828,7 @@
       </c>
     </row>
     <row r="125" spans="1:10" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A125" s="71"/>
+      <c r="A125" s="74"/>
       <c r="B125" s="29">
         <v>124</v>
       </c>
@@ -38854,7 +38854,7 @@
       </c>
     </row>
     <row r="126" spans="1:10" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A126" s="71"/>
+      <c r="A126" s="74"/>
       <c r="B126" s="29">
         <v>125</v>
       </c>
@@ -38880,7 +38880,7 @@
       </c>
     </row>
     <row r="127" spans="1:10" ht="51" x14ac:dyDescent="0.3">
-      <c r="A127" s="71"/>
+      <c r="A127" s="74"/>
       <c r="B127" s="29">
         <v>126</v>
       </c>
@@ -38906,7 +38906,7 @@
       </c>
     </row>
     <row r="128" spans="1:10" ht="41.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="72"/>
+      <c r="A128" s="79"/>
       <c r="B128" s="53">
         <v>127</v>
       </c>
@@ -38932,7 +38932,7 @@
       </c>
     </row>
     <row r="129" spans="1:10" ht="51" x14ac:dyDescent="0.3">
-      <c r="A129" s="76" t="s">
+      <c r="A129" s="70" t="s">
         <v>371</v>
       </c>
       <c r="B129" s="54">
@@ -38960,7 +38960,7 @@
       </c>
     </row>
     <row r="130" spans="1:10" ht="51" x14ac:dyDescent="0.3">
-      <c r="A130" s="77"/>
+      <c r="A130" s="71"/>
       <c r="B130" s="30">
         <v>129</v>
       </c>
@@ -38986,7 +38986,7 @@
       </c>
     </row>
     <row r="131" spans="1:10" ht="51" x14ac:dyDescent="0.3">
-      <c r="A131" s="77"/>
+      <c r="A131" s="71"/>
       <c r="B131" s="30">
         <v>130</v>
       </c>
@@ -39012,7 +39012,7 @@
       </c>
     </row>
     <row r="132" spans="1:10" ht="51" x14ac:dyDescent="0.3">
-      <c r="A132" s="77"/>
+      <c r="A132" s="71"/>
       <c r="B132" s="29">
         <v>131</v>
       </c>
@@ -39040,7 +39040,7 @@
       </c>
     </row>
     <row r="133" spans="1:10" ht="51" x14ac:dyDescent="0.3">
-      <c r="A133" s="77"/>
+      <c r="A133" s="71"/>
       <c r="B133" s="30">
         <v>132</v>
       </c>
@@ -39064,7 +39064,7 @@
       <c r="J133" s="24"/>
     </row>
     <row r="134" spans="1:10" ht="51" x14ac:dyDescent="0.3">
-      <c r="A134" s="77"/>
+      <c r="A134" s="71"/>
       <c r="B134" s="29">
         <v>133</v>
       </c>
@@ -39090,7 +39090,7 @@
       </c>
     </row>
     <row r="135" spans="1:10" ht="71.400000000000006" x14ac:dyDescent="0.3">
-      <c r="A135" s="77"/>
+      <c r="A135" s="71"/>
       <c r="B135" s="29">
         <v>134</v>
       </c>
@@ -39116,7 +39116,7 @@
       </c>
     </row>
     <row r="136" spans="1:10" ht="41.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="78"/>
+      <c r="A136" s="72"/>
       <c r="B136" s="31">
         <v>135</v>
       </c>
@@ -39142,7 +39142,7 @@
       </c>
     </row>
     <row r="137" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A137" s="76" t="s">
+      <c r="A137" s="70" t="s">
         <v>397</v>
       </c>
       <c r="B137" s="55">
@@ -39170,7 +39170,7 @@
       </c>
     </row>
     <row r="138" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="77"/>
+      <c r="A138" s="71"/>
       <c r="B138" s="29">
         <v>137</v>
       </c>
@@ -39196,7 +39196,7 @@
       </c>
     </row>
     <row r="139" spans="1:10" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A139" s="77"/>
+      <c r="A139" s="71"/>
       <c r="B139" s="29">
         <v>138</v>
       </c>
@@ -39222,7 +39222,7 @@
       </c>
     </row>
     <row r="140" spans="1:10" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="78"/>
+      <c r="A140" s="72"/>
       <c r="B140" s="56">
         <v>139</v>
       </c>
@@ -39248,7 +39248,7 @@
       </c>
     </row>
     <row r="141" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A141" s="76" t="s">
+      <c r="A141" s="70" t="s">
         <v>410</v>
       </c>
       <c r="B141" s="32">
@@ -39276,7 +39276,7 @@
       </c>
     </row>
     <row r="142" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A142" s="77"/>
+      <c r="A142" s="71"/>
       <c r="B142" s="29">
         <v>141</v>
       </c>
@@ -39302,7 +39302,7 @@
       </c>
     </row>
     <row r="143" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A143" s="77"/>
+      <c r="A143" s="71"/>
       <c r="B143" s="29">
         <v>142</v>
       </c>
@@ -39328,7 +39328,7 @@
       </c>
     </row>
     <row r="144" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A144" s="77"/>
+      <c r="A144" s="71"/>
       <c r="B144" s="29">
         <v>143</v>
       </c>
@@ -39354,7 +39354,7 @@
       </c>
     </row>
     <row r="145" spans="1:10" ht="61.2" x14ac:dyDescent="0.3">
-      <c r="A145" s="77"/>
+      <c r="A145" s="71"/>
       <c r="B145" s="29">
         <v>144</v>
       </c>
@@ -39380,7 +39380,7 @@
       </c>
     </row>
     <row r="146" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A146" s="77"/>
+      <c r="A146" s="71"/>
       <c r="B146" s="30">
         <v>119145</v>
       </c>
@@ -39406,7 +39406,7 @@
       </c>
     </row>
     <row r="147" spans="1:10" ht="71.400000000000006" x14ac:dyDescent="0.3">
-      <c r="A147" s="77"/>
+      <c r="A147" s="71"/>
       <c r="B147" s="29">
         <v>120146</v>
       </c>
@@ -39432,7 +39432,7 @@
       </c>
     </row>
     <row r="148" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A148" s="77"/>
+      <c r="A148" s="71"/>
       <c r="B148" s="59">
         <v>147</v>
       </c>
@@ -39458,7 +39458,7 @@
       </c>
     </row>
     <row r="149" spans="1:10" ht="153.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="77"/>
+      <c r="A149" s="71"/>
       <c r="B149" s="57">
         <v>148</v>
       </c>
@@ -39484,7 +39484,7 @@
       </c>
     </row>
     <row r="150" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A150" s="70" t="s">
+      <c r="A150" s="73" t="s">
         <v>421</v>
       </c>
       <c r="B150" s="32">
@@ -39507,10 +39507,12 @@
         <v>424</v>
       </c>
       <c r="I150" s="15"/>
-      <c r="J150" s="44"/>
+      <c r="J150" s="44" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="151" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A151" s="71"/>
+      <c r="A151" s="74"/>
       <c r="B151" s="29">
         <v>150</v>
       </c>
@@ -39531,10 +39533,12 @@
         <v>61</v>
       </c>
       <c r="I151" s="7"/>
-      <c r="J151" s="24"/>
+      <c r="J151" s="24" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="152" spans="1:10" ht="173.4" x14ac:dyDescent="0.3">
-      <c r="A152" s="71"/>
+      <c r="A152" s="74"/>
       <c r="B152" s="29">
         <v>151</v>
       </c>
@@ -39555,10 +39559,12 @@
         <v>60</v>
       </c>
       <c r="I152" s="7"/>
-      <c r="J152" s="24"/>
+      <c r="J152" s="24" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="153" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A153" s="71"/>
+      <c r="A153" s="74"/>
       <c r="B153" s="29">
         <v>152</v>
       </c>
@@ -39579,10 +39585,12 @@
         <v>531</v>
       </c>
       <c r="I153" s="7"/>
-      <c r="J153" s="24"/>
+      <c r="J153" s="24" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="154" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A154" s="71"/>
+      <c r="A154" s="74"/>
       <c r="B154" s="29">
         <v>153</v>
       </c>
@@ -39603,10 +39611,12 @@
         <v>429</v>
       </c>
       <c r="I154" s="7"/>
-      <c r="J154" s="24"/>
+      <c r="J154" s="24" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="155" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A155" s="71"/>
+      <c r="A155" s="74"/>
       <c r="B155" s="29">
         <v>154</v>
       </c>
@@ -39627,10 +39637,12 @@
         <v>432</v>
       </c>
       <c r="I155" s="7"/>
-      <c r="J155" s="24"/>
+      <c r="J155" s="24" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="156" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A156" s="71"/>
+      <c r="A156" s="74"/>
       <c r="B156" s="29">
         <v>155</v>
       </c>
@@ -39654,7 +39666,7 @@
       <c r="J156" s="24"/>
     </row>
     <row r="157" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A157" s="71"/>
+      <c r="A157" s="74"/>
       <c r="B157" s="29">
         <v>156</v>
       </c>
@@ -39675,10 +39687,12 @@
         <v>541</v>
       </c>
       <c r="I157" s="7"/>
-      <c r="J157" s="24"/>
+      <c r="J157" s="24" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="158" spans="1:10" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A158" s="71"/>
+      <c r="A158" s="74"/>
       <c r="B158" s="29">
         <v>157</v>
       </c>
@@ -39699,10 +39713,12 @@
         <v>545</v>
       </c>
       <c r="I158" s="7"/>
-      <c r="J158" s="24"/>
+      <c r="J158" s="24" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="159" spans="1:10" ht="143.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A159" s="72"/>
+      <c r="A159" s="79"/>
       <c r="B159" s="56">
         <v>158</v>
       </c>
@@ -39723,7 +39739,9 @@
         <v>437</v>
       </c>
       <c r="I159" s="27"/>
-      <c r="J159" s="28"/>
+      <c r="J159" s="28" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C160" s="47"/>
@@ -39731,6 +39749,14 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A150:A159"/>
+    <mergeCell ref="A83:A91"/>
+    <mergeCell ref="A129:A136"/>
+    <mergeCell ref="A137:A140"/>
+    <mergeCell ref="A141:A149"/>
+    <mergeCell ref="A108:A121"/>
+    <mergeCell ref="A122:A128"/>
+    <mergeCell ref="A92:A107"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A42:A50"/>
     <mergeCell ref="A51:A63"/>
@@ -39742,14 +39768,6 @@
     <mergeCell ref="A25:A28"/>
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A35:A41"/>
-    <mergeCell ref="A150:A159"/>
-    <mergeCell ref="A83:A91"/>
-    <mergeCell ref="A129:A136"/>
-    <mergeCell ref="A137:A140"/>
-    <mergeCell ref="A141:A149"/>
-    <mergeCell ref="A108:A121"/>
-    <mergeCell ref="A122:A128"/>
-    <mergeCell ref="A92:A107"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>